<commit_message>
Add percent change graph
</commit_message>
<xml_diff>
--- a/COP-6616-Final-Project-Scenario-1/docs/scenario_1_graphs.xlsx
+++ b/COP-6616-Final-Project-Scenario-1/docs/scenario_1_graphs.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\UCF\UCF Year 7\COP-6616-Final-Project\COP-6616-Final-Project-Scenario-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA797AE2-5627-4E0E-A031-BD0863A99EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FB478A-EE7B-4483-BF04-3B21F3856257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{44B590F9-641C-46CB-B2DD-1B7EC7A4B0D1}"/>
   </bookViews>
@@ -18,7 +18,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>TX buffer size</t>
   </si>
@@ -86,12 +87,31 @@
   <si>
     <t>Sum of Throughput (MB/sec)</t>
   </si>
+  <si>
+    <t>Percent change</t>
+  </si>
+  <si>
+    <t>Percent change is speedup from memcpy to DMA</t>
+  </si>
+  <si>
+    <t>Values &lt; 1 are slowdown</t>
+  </si>
+  <si>
+    <t>Sum of Percent change</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,22 +137,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6565"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1906,6 +1934,494 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[scenario_1_graphs.xlsx]Graphs!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$B$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$A$60:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$B$60:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.5442448436460412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.47231833910034604</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.43982407037185123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.30668380462724931</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.18433678997059277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32926217165802241</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36510571378647572</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35241745145234038</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FF6565"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F1CA-499B-B0F4-4A739806855B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="267273839"/>
+        <c:axId val="267274319"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="267273839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>Transfer Size (words)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267274319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="267274319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1"/>
+                  <a:t>Percent improvement</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267273839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1946,7 +2462,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2523,6 +3582,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E56EBB-C88E-92F0-64C8-2B6BDBF280DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2558,6 +3653,36 @@
     </cacheField>
     <cacheField name="Throughput (MB/sec)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.0608886393878905" maxValue="18.530597722960152"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ethan Thomas" refreshedDate="45977.892905555556" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{53E2F69E-6D5E-4C17-A530-A9E3143ABBEC}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="K1:L9" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="TX buffer size" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="16" maxValue="2048" count="8">
+        <n v="2048"/>
+        <n v="1024"/>
+        <n v="512"/>
+        <n v="256"/>
+        <n v="128"/>
+        <n v="64"/>
+        <n v="32"/>
+        <n v="16"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Percent change" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.5442448436460412" maxValue="0.36510571378647572"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -2685,8 +3810,306 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <x v="0"/>
+    <n v="0.35241745145234038"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0.36510571378647572"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="0.32926217165802241"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="-0.18433678997059277"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="-0.30668380462724931"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="-0.43982407037185123"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="-0.47231833910034604"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="-0.5442448436460412"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1249E34A-AC1B-4BDE-9592-CCE32E93B475}" name="PivotTable11" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="15">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECE93EA2-7E5C-41EF-B7FC-C7680717BE30}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+  <location ref="A3:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="9">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Frequency (Hz)" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="1" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5E56533-E96F-4E35-A0C6-ADC8B331FE6F}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A59:B68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Percent change" fld="1" baseField="0" baseItem="0" numFmtId="9"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1249E34A-AC1B-4BDE-9592-CCE32E93B475}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
   <location ref="A33:D43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -2873,169 +4296,6 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ECE93EA2-7E5C-41EF-B7FC-C7680717BE30}" name="PivotTable10" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
-  <location ref="A3:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="9">
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" sortType="descending">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Frequency (Hz)" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="1" format="16" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="17" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="18" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="20" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="21" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -3370,10 +4630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67EBC8C-CD68-40A7-B0CE-FA25E2321076}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,9 +4643,12 @@
     <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3404,8 +4667,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2048</v>
       </c>
@@ -3426,8 +4698,18 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <v>2048</v>
+      </c>
+      <c r="L2" s="3">
+        <f>C2/C3-1</f>
+        <v>0.35241745145234038</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2048</v>
       </c>
@@ -3448,8 +4730,15 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
+      <c r="K3">
+        <v>1024</v>
+      </c>
+      <c r="L3" s="3">
+        <f>C4/C5-1</f>
+        <v>0.36510571378647572</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1024</v>
       </c>
@@ -3470,8 +4759,15 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
+      <c r="K4">
+        <v>512</v>
+      </c>
+      <c r="L4" s="3">
+        <f>C6/C7-1</f>
+        <v>0.32926217165802241</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1024</v>
       </c>
@@ -3492,8 +4788,15 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
+      <c r="K5">
+        <v>256</v>
+      </c>
+      <c r="L5" s="3">
+        <f>C8/C9-1</f>
+        <v>-0.18433678997059277</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>512</v>
       </c>
@@ -3514,8 +4817,15 @@
       <c r="F6" t="s">
         <v>6</v>
       </c>
+      <c r="K6">
+        <v>128</v>
+      </c>
+      <c r="L6" s="3">
+        <f>C10/C11-1</f>
+        <v>-0.30668380462724931</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>512</v>
       </c>
@@ -3536,8 +4846,15 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
+      <c r="K7">
+        <v>64</v>
+      </c>
+      <c r="L7" s="3">
+        <f>C12/C13-1</f>
+        <v>-0.43982407037185123</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>256</v>
       </c>
@@ -3558,8 +4875,15 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
+      <c r="K8">
+        <v>32</v>
+      </c>
+      <c r="L8" s="3">
+        <f>C14/C15-1</f>
+        <v>-0.47231833910034604</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>256</v>
       </c>
@@ -3580,8 +4904,15 @@
       <c r="F9" t="s">
         <v>6</v>
       </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9" s="3">
+        <f>C16/C17-1</f>
+        <v>-0.5442448436460412</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>128</v>
       </c>
@@ -3603,7 +4934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>128</v>
       </c>
@@ -3625,7 +4956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>64</v>
       </c>
@@ -3647,7 +4978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>64</v>
       </c>
@@ -3669,7 +5000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32</v>
       </c>
@@ -3691,7 +5022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32</v>
       </c>
@@ -3713,7 +5044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3764,16 +5095,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A84A40-95E9-44B0-90D9-3F510A203314}">
-  <dimension ref="A3:D43"/>
+  <dimension ref="A3:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="W77" sqref="W77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -3811,13 +5142,13 @@
       <c r="A5" s="2">
         <v>16</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>145985.40145985401</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>66533.599467731197</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>212519.00092758521</v>
       </c>
     </row>
@@ -3825,13 +5156,13 @@
       <c r="A6" s="2">
         <v>32</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>109289.61748633879</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>57670.126874279122</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>166959.74436061791</v>
       </c>
     </row>
@@ -3839,13 +5170,13 @@
       <c r="A7" s="2">
         <v>64</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>71377.587437544615</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>39984.006397441022</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>111361.59383498563</v>
       </c>
     </row>
@@ -3853,13 +5184,13 @@
       <c r="A8" s="2">
         <v>128</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>37078.23507601038</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>25706.940874035987</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>62785.175950046367</v>
       </c>
     </row>
@@ -3867,13 +5198,13 @@
       <c r="A9" s="2">
         <v>256</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>18975.332068311196</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>15477.480266212659</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>34452.812334523856</v>
       </c>
     </row>
@@ -3881,13 +5212,13 @@
       <c r="A10" s="2">
         <v>512</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>6293.2662051604775</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>8365.4007026936597</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>14658.666907854138</v>
       </c>
     </row>
@@ -3895,13 +5226,13 @@
       <c r="A11" s="2">
         <v>1024</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>3200</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>4368.3382841167222</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>7568.3382841167222</v>
       </c>
     </row>
@@ -3909,13 +5240,13 @@
       <c r="A12" s="2">
         <v>2048</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>1727.8916266371773</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>2336.8307900824898</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>4064.7224167196673</v>
       </c>
     </row>
@@ -3923,13 +5254,13 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>393927.3313598567</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>220442.72365659289</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>614370.05501644954</v>
       </c>
     </row>
@@ -3959,13 +5290,13 @@
       <c r="A35" s="2">
         <v>16</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35">
         <v>8.9102417883211675</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35">
         <v>4.0608886393878905</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35">
         <v>12.971130427709058</v>
       </c>
     </row>
@@ -3973,13 +5304,13 @@
       <c r="A36" s="2">
         <v>32</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36">
         <v>13.34101775956284</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36">
         <v>7.0398104094579006</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36">
         <v>20.380828169020742</v>
       </c>
     </row>
@@ -3987,13 +5318,13 @@
       <c r="A37" s="2">
         <v>64</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>17.426168807994291</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37">
         <v>9.7617203118752496</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37">
         <v>27.187889119869538</v>
       </c>
     </row>
@@ -4001,13 +5332,13 @@
       <c r="A38" s="2">
         <v>128</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>18.104606970708193</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38">
         <v>12.552217223650384</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38">
         <v>30.656824194358578</v>
       </c>
     </row>
@@ -4015,13 +5346,13 @@
       <c r="A39" s="2">
         <v>256</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>18.530597722960152</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39">
         <v>15.114726822473299</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39">
         <v>33.645324545433454</v>
       </c>
     </row>
@@ -4029,13 +5360,13 @@
       <c r="A40" s="2">
         <v>512</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>12.291535556954058</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40">
         <v>16.338673247448554</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40">
         <v>28.630208804402614</v>
       </c>
     </row>
@@ -4043,13 +5374,13 @@
       <c r="A41" s="2">
         <v>1024</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41">
         <v>12.5</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41">
         <v>17.063821422330946</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41">
         <v>29.563821422330946</v>
       </c>
     </row>
@@ -4057,13 +5388,13 @@
       <c r="A42" s="2">
         <v>2048</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42">
         <v>13.499153333102948</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42">
         <v>18.256490547519451</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42">
         <v>31.755643880622401</v>
       </c>
     </row>
@@ -4071,18 +5402,98 @@
       <c r="A43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>114.60332193960366</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>100.18834862414367</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43">
         <v>214.79167056374735</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>16</v>
+      </c>
+      <c r="B60" s="4">
+        <v>-0.5442448436460412</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>32</v>
+      </c>
+      <c r="B61" s="4">
+        <v>-0.47231833910034604</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>64</v>
+      </c>
+      <c r="B62" s="4">
+        <v>-0.43982407037185123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>128</v>
+      </c>
+      <c r="B63" s="4">
+        <v>-0.30668380462724931</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>256</v>
+      </c>
+      <c r="B64" s="4">
+        <v>-0.18433678997059277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>512</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0.32926217165802241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.36510571378647572</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>2048</v>
+      </c>
+      <c r="B67" s="4">
+        <v>0.35241745145234038</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" s="4">
+        <v>-0.90062251081924205</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>